<commit_message>
feat: create user in progress
</commit_message>
<xml_diff>
--- a/visitors.xlsx
+++ b/visitors.xlsx
@@ -1,43 +1,113 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\face-recognition\face-recognition-backend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91125BCC-F76D-4217-B88B-1B2647144A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>CNIC</t>
+  </si>
+  <si>
+    <t>Check-in</t>
+  </si>
+  <si>
+    <t>Check-out</t>
+  </si>
+  <si>
+    <t>Aqib</t>
+  </si>
+  <si>
+    <t>42301-2474477-5</t>
+  </si>
+  <si>
+    <t>2025-04-24 18:20:59 | 2025-04-25 15:46:33 | 2025-04-25 15:47:18</t>
+  </si>
+  <si>
+    <t>mohsin</t>
+  </si>
+  <si>
+    <t>42301123456789</t>
+  </si>
+  <si>
+    <t>2025-04-24 18:21:36 | 2025-04-25 15:41:25 | 2025-04-25 15:47:53</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>42201-0916837-9</t>
+  </si>
+  <si>
+    <t>2025-04-25 15:41:24 | 2025-04-25 15:47:52</t>
+  </si>
+  <si>
+    <t>zubair</t>
+  </si>
+  <si>
+    <t>1234556778890</t>
+  </si>
+  <si>
+    <t>2025-04-25 15:41:51</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,94 +115,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,114 +428,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>CNIC</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Check-in</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Check-out</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Aqib</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>42301-2474477-5</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-04-24 18:20:59 | 2025-04-25 15:46:33 | 2025-04-25 15:47:18</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>mohsin</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>42301123456789</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-04-24 18:21:36 | 2025-04-25 15:41:25 | 2025-04-25 15:47:53</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>42201-0916837-9</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-04-25 15:41:24 | 2025-04-25 15:47:52</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>zubair</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1234556778890</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-04-25 15:41:51</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: created api of create user
</commit_message>
<xml_diff>
--- a/visitors.xlsx
+++ b/visitors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\face-recognition\face-recognition-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91125BCC-F76D-4217-B88B-1B2647144A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2389D1AB-8621-458F-BED0-3240D2CB684F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>CNIC</t>
-  </si>
-  <si>
-    <t>Check-in</t>
-  </si>
-  <si>
-    <t>Check-out</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>full_name</t>
+  </si>
+  <si>
+    <t>cnic</t>
+  </si>
+  <si>
+    <t>check_in</t>
+  </si>
+  <si>
+    <t>check_out</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
   <si>
     <t>Aqib</t>
@@ -70,7 +73,16 @@
     <t>2025-04-25 15:41:51</t>
   </si>
   <si>
-    <t>Id</t>
+    <t>aahil alwani</t>
+  </si>
+  <si>
+    <t>42w322e633333</t>
+  </si>
+  <si>
+    <t>1232536327</t>
+  </si>
+  <si>
+    <t>30 apr 2025 1:02pm |</t>
   </si>
 </sst>
 </file>
@@ -429,21 +441,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,55 +470,69 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add create-visitor api, add logic of saving checkin and checkout time
</commit_message>
<xml_diff>
--- a/visitors.xlsx
+++ b/visitors.xlsx
@@ -1,119 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\face-recognition\face-recognition-backend\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2389D1AB-8621-458F-BED0-3240D2CB684F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>full_name</t>
-  </si>
-  <si>
-    <t>cnic</t>
-  </si>
-  <si>
-    <t>check_in</t>
-  </si>
-  <si>
-    <t>check_out</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>Aqib</t>
-  </si>
-  <si>
-    <t>42301-2474477-5</t>
-  </si>
-  <si>
-    <t>2025-04-24 18:20:59 | 2025-04-25 15:46:33 | 2025-04-25 15:47:18</t>
-  </si>
-  <si>
-    <t>mohsin</t>
-  </si>
-  <si>
-    <t>42301123456789</t>
-  </si>
-  <si>
-    <t>2025-04-24 18:21:36 | 2025-04-25 15:41:25 | 2025-04-25 15:47:53</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>42201-0916837-9</t>
-  </si>
-  <si>
-    <t>2025-04-25 15:41:24 | 2025-04-25 15:47:52</t>
-  </si>
-  <si>
-    <t>zubair</t>
-  </si>
-  <si>
-    <t>1234556778890</t>
-  </si>
-  <si>
-    <t>2025-04-25 15:41:51</t>
-  </si>
-  <si>
-    <t>aahil alwani</t>
-  </si>
-  <si>
-    <t>42w322e633333</t>
-  </si>
-  <si>
-    <t>1232536327</t>
-  </si>
-  <si>
-    <t>30 apr 2025 1:02pm |</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -132,27 +59,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -440,95 +426,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col width="10.6640625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="15.44140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="56.44140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="18.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>full_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cnic</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>check_in</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>check_out</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Aqib</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>42301-2474477-5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-04-24 18:20:59 | 2025-04-25 15:46:33 | 2025-04-25 15:47:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mohsin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>42301123456789</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-04-24 18:21:36 | 2025-04-25 15:41:25 | 2025-04-25 15:47:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>42201-0916837-9</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-04-25 15:41:24 | 2025-04-25 15:47:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>zubair</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1234556778890</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-04-25 15:41:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>aahil alwani</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>42w322e633333</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>30 apr 2025 1:02pm |</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1232536327</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>aahil alwani</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>42w322e633333</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>30 apr 2025 1:02pm |</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1232536327</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>aahil alwani</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>42w322e633333</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>30 apr 2025 1:02pm |</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1232536327</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Aahil Alwani</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>4220104764125</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-05-01T21:00:20.857Z</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>321453627e8r9rqwefywdeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>aahilaaaa</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>4220104764125</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-05-02T05:04:07.581Z</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>321453627e8r9rqwefywdeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>qvgqwydwyus</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>4220104764125</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-05-02T05:07:47.264Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>sanjay</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>4220104764125</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-05-02T05:14:03.919Z</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>c53cc042-a1ee-4e08-a755-2bad852b5ee0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Aqib</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>4220104764125</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-05-02T05:22:10.898Z</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>9e749a7c-2e46-4ff5-ad1f-1123026545af</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: add user name in checkout
</commit_message>
<xml_diff>
--- a/visitors.xlsx
+++ b/visitors.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -521,7 +521,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-05-02T11:32:00.422Z</t>
+          <t>2025-05-02T11:32:00.422Z | 2025-05-05T08:08:42.144672Z</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -532,6 +532,33 @@
       <c r="E4" t="inlineStr">
         <is>
           <t>ff476071-f5d9-42da-b64c-4113d5b38cba</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Aahil Alwani</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4220109168379</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-05-05T08:18:11.498Z | 2025-05-05T08:19:42.748438Z | 2025-05-05T08:49:27.254322Z</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-05-05T08:51:19.823867Z | 2025-05-05T08:53:50.148984Z</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>abbcad36-1f96-4c68-a2a2-ef484605714c</t>
         </is>
       </c>
     </row>

</xml_diff>